<commit_message>
update packed bubble chart
</commit_message>
<xml_diff>
--- a/data/minerals.xlsx
+++ b/data/minerals.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlnphng/Documents/FIT3179/A2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5A33AB-0F77-BB47-8733-17948C298A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E760C37-3FB0-F34C-A0C3-715191E15907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2500" windowWidth="26440" windowHeight="13980" xr2:uid="{D9814B64-A5DD-3E41-B078-325FAC711387}"/>
+    <workbookView xWindow="1980" yWindow="2460" windowWidth="26440" windowHeight="13980" xr2:uid="{D9814B64-A5DD-3E41-B078-325FAC711387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Iron Ore</t>
   </si>
@@ -53,7 +53,25 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Other</t>
+    <t>Other Mineral</t>
+  </si>
+  <si>
+    <t>Manganese Ore</t>
+  </si>
+  <si>
+    <t>Copper Ore</t>
+  </si>
+  <si>
+    <t>Aluminium Ore</t>
+  </si>
+  <si>
+    <t>Zinc Ore</t>
+  </si>
+  <si>
+    <t>Precious Metal Ore</t>
+  </si>
+  <si>
+    <t>Crude Petroleum</t>
   </si>
 </sst>
 </file>
@@ -425,16 +443,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5175D2F-BF12-1443-BB42-47A4D1C4448E}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -447,18 +465,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>80750673208</v>
+        <v>109.095566316</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>37477829782</v>
+        <v>87.851720001000004</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -466,7 +484,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>27029973762</v>
+        <v>67.328487191999997</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -474,12 +492,60 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>15899255736</v>
+        <v>8.2697793009999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>7.5440299729999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>4.8912432130000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>2.2128310440000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1.562934727</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>1.388132554</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.86498837700000009</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B65">
-    <sortCondition descending="1" ref="B1:B65"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
+    <sortCondition descending="1" ref="B1:B11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated year filter to section 4
</commit_message>
<xml_diff>
--- a/data/minerals.xlsx
+++ b/data/minerals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlnphng/Documents/FIT3179/A2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E760C37-3FB0-F34C-A0C3-715191E15907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBF97CE-B9DE-5F4E-AEA3-AEC490A995A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2460" windowWidth="26440" windowHeight="13980" xr2:uid="{D9814B64-A5DD-3E41-B078-325FAC711387}"/>
+    <workbookView xWindow="8960" yWindow="560" windowWidth="26440" windowHeight="15900" xr2:uid="{D9814B64-A5DD-3E41-B078-325FAC711387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Iron Ore</t>
-  </si>
-  <si>
-    <t>Coal Briquettes</t>
-  </si>
-  <si>
-    <t>Petroleum Gas</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="11">
   <si>
     <t>Type</t>
   </si>
@@ -53,35 +44,48 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Other Mineral</t>
-  </si>
-  <si>
-    <t>Manganese Ore</t>
-  </si>
-  <si>
-    <t>Copper Ore</t>
-  </si>
-  <si>
-    <t>Aluminium Ore</t>
-  </si>
-  <si>
-    <t>Zinc Ore</t>
-  </si>
-  <si>
-    <t>Precious Metal Ore</t>
-  </si>
-  <si>
-    <t>Crude Petroleum</t>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Petrol Gas</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>Zinc</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>Al</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,8 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,109 +449,488 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5175D2F-BF12-1443-BB42-47A4D1C4448E}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1">
+        <v>109.095566316</v>
+      </c>
+      <c r="C2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>109.095566316</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>87.851720001000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
         <v>67.328487191999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
         <v>8.2697793009999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>7.5440299729999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4.8912432130000001</v>
+      </c>
+      <c r="C6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>4.8912432130000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.2128310440000001</v>
+      </c>
+      <c r="C7">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
-        <v>2.2128310440000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>1.388132554</v>
+      </c>
+      <c r="C8">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>1.562934727</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B9" s="1">
+        <v>0.86498837700000009</v>
+      </c>
+      <c r="C9">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>118.255775691</v>
+      </c>
+      <c r="C10">
+        <v>2021</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>56.459034072000001</v>
+      </c>
+      <c r="C11">
+        <v>2021</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>39.877070193000002</v>
+      </c>
+      <c r="C12">
+        <v>2021</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.8224322470000001</v>
+      </c>
+      <c r="C13">
+        <v>2021</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2.005842592</v>
+      </c>
+      <c r="C14">
+        <v>2021</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.356501451</v>
+      </c>
+      <c r="C15">
+        <v>2021</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B10">
-        <v>1.388132554</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B16" s="1">
+        <v>1.2096123030000001</v>
+      </c>
+      <c r="C16">
+        <v>2021</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.99534338299999991</v>
+      </c>
+      <c r="C17">
+        <v>2021</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <v>80.750673207999995</v>
+      </c>
+      <c r="C18">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>37.477829782000001</v>
+      </c>
+      <c r="C19">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
+        <v>27.029973762000001</v>
+      </c>
+      <c r="C20">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.868088593</v>
+      </c>
+      <c r="C21">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>0.86498837700000009</v>
+      <c r="B22" s="1">
+        <v>1.4007187670000001</v>
+      </c>
+      <c r="C22">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.1753053659999999</v>
+      </c>
+      <c r="C23">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.075121851</v>
+      </c>
+      <c r="C24">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.63952626599999995</v>
+      </c>
+      <c r="C25">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>679.82343710999999</v>
+      </c>
+      <c r="C26">
+        <v>2019</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1">
+        <v>522.78945810000005</v>
+      </c>
+      <c r="C27">
+        <v>2019</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1">
+        <v>343.68508125</v>
+      </c>
+      <c r="C28">
+        <v>2019</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45.975928940000003</v>
+      </c>
+      <c r="C29">
+        <v>2019</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1">
+        <v>16.620421090000001</v>
+      </c>
+      <c r="C30">
+        <v>2019</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1">
+        <v>15.862939219999998</v>
+      </c>
+      <c r="C31">
+        <v>2019</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1">
+        <v>11.517813459999998</v>
+      </c>
+      <c r="C32">
+        <v>2019</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1">
+        <v>9.7585685800000004</v>
+      </c>
+      <c r="C33">
+        <v>2019</v>
+      </c>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="1">
+        <v>580.94072911000001</v>
+      </c>
+      <c r="C34">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1">
+        <v>483.85886627000002</v>
+      </c>
+      <c r="C35">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1">
+        <v>315.74598829000001</v>
+      </c>
+      <c r="C36">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45.120194589999997</v>
+      </c>
+      <c r="C37">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1">
+        <v>19.318038659999999</v>
+      </c>
+      <c r="C38">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="1">
+        <v>19.15634755</v>
+      </c>
+      <c r="C39">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="1">
+        <v>11.957596819999999</v>
+      </c>
+      <c r="C40">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="1">
+        <v>10.162372300000001</v>
+      </c>
+      <c r="C41">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
-    <sortCondition descending="1" ref="B1:B11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B9">
+    <sortCondition descending="1" ref="B1:B9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update on minerals csv
</commit_message>
<xml_diff>
--- a/data/minerals.xlsx
+++ b/data/minerals.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlnphng/Documents/FIT3179/A2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBF97CE-B9DE-5F4E-AEA3-AEC490A995A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6C5E53C-5859-4E49-B340-87FEC5D6E848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="560" windowWidth="26440" windowHeight="15900" xr2:uid="{D9814B64-A5DD-3E41-B078-325FAC711387}"/>
+    <workbookView xWindow="1180" yWindow="560" windowWidth="26440" windowHeight="15900" xr2:uid="{D9814B64-A5DD-3E41-B078-325FAC711387}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="minerals" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -451,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5175D2F-BF12-1443-BB42-47A4D1C4448E}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>

</xml_diff>